<commit_message>
maj bdd + alertes
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/centres_candidature_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/centres_candidature_template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hergalan6\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE723FE-B601-4958-84B4-32B3DFD8274F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="4185" windowWidth="18555" windowHeight="5610"/>
+    <workbookView xWindow="1890" yWindow="4185" windowWidth="18555" windowHeight="5610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="formations" sheetId="1" r:id="rId1"/>
@@ -43,9 +49,6 @@
     <t>Parmétrage décision</t>
   </si>
   <si>
-    <t>Copie des mails (BCC)</t>
-  </si>
-  <si>
     <t>Mail contact</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
     <t>${ctr.temParam}</t>
   </si>
   <si>
-    <t>${ctr.temSendMail}</t>
-  </si>
-  <si>
     <t>${ctr.mailContact}</t>
   </si>
   <si>
@@ -188,12 +188,18 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Type de réception de copie des mails (BCC)</t>
+  </si>
+  <si>
+    <t>${ctr.typSendMailCtrCand}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -258,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -270,6 +276,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,6 +294,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -333,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,9 +378,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -401,6 +430,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,7 +622,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -592,7 +639,7 @@
     <col min="4" max="4" width="22.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47" style="3" customWidth="1"/>
     <col min="8" max="8" width="26.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="30" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" style="3" customWidth="1"/>
@@ -618,70 +665,70 @@
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>3</v>
@@ -698,101 +745,101 @@
     </row>
     <row r="2" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="5"/>

</xml_diff>